<commit_message>
Updated Plot For The Comparative Analysis
</commit_message>
<xml_diff>
--- a/Compare_ILS_and_SA/Analysis.xlsx
+++ b/Compare_ILS_and_SA/Analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sello Tebogo\Documents\Submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{209B5DD4-332A-41D8-ACA8-DB854F58874C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBF6986-09C7-4563-ABAE-01FE2238EF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{040D34DC-8274-4C49-9F13-F233A2CADE55}"/>
   </bookViews>
@@ -157,7 +157,7 @@
                 </a:solidFill>
                 <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t>Critical Comparative Analysis</a:t>
+              <a:t>Graphical Plot Representation of Results</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2881,6 +2881,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-ZA" sz="1800"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-ZA" sz="1800" baseline="0"/>
+                  <a:t> of Iterations</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-ZA" sz="1800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2943,6 +3003,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>Objective Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3627,16 +3742,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1905</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>175259</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>137</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>232410</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>173354</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3963,8 +4078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7CF48E2-A5B2-4AE5-86B9-84E022EB968B}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="V144" sqref="V144"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4009,7 +4124,7 @@
         <v>88</v>
       </c>
       <c r="E2">
-        <f>81</f>
+        <f>MIN(B2, C2)</f>
         <v>81</v>
       </c>
     </row>
@@ -4029,7 +4144,7 @@
         <v>88</v>
       </c>
       <c r="E3">
-        <f>81</f>
+        <f>MIN(E2,MIN(B3:C3))</f>
         <v>81</v>
       </c>
     </row>
@@ -4049,7 +4164,7 @@
         <v>95</v>
       </c>
       <c r="E4">
-        <f>81</f>
+        <f t="shared" ref="E4:E67" si="2">MIN(E3,MIN(B4:C4))</f>
         <v>81</v>
       </c>
     </row>
@@ -4069,7 +4184,7 @@
         <v>95</v>
       </c>
       <c r="E5">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4089,7 +4204,7 @@
         <v>88.5</v>
       </c>
       <c r="E6">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4109,7 +4224,7 @@
         <v>92.5</v>
       </c>
       <c r="E7">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4129,7 +4244,7 @@
         <v>108</v>
       </c>
       <c r="E8">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4149,7 +4264,7 @@
         <v>96.5</v>
       </c>
       <c r="E9">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4169,7 +4284,7 @@
         <v>107.5</v>
       </c>
       <c r="E10">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4189,7 +4304,7 @@
         <v>100.5</v>
       </c>
       <c r="E11">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4209,7 +4324,7 @@
         <v>92.5</v>
       </c>
       <c r="E12">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4229,7 +4344,7 @@
         <v>95</v>
       </c>
       <c r="E13">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4249,7 +4364,7 @@
         <v>88</v>
       </c>
       <c r="E14">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4269,7 +4384,7 @@
         <v>91</v>
       </c>
       <c r="E15">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4289,7 +4404,7 @@
         <v>91</v>
       </c>
       <c r="E16">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4309,7 +4424,7 @@
         <v>93.5</v>
       </c>
       <c r="E17">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4329,7 +4444,7 @@
         <v>100.5</v>
       </c>
       <c r="E18">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4349,7 +4464,7 @@
         <v>86.5</v>
       </c>
       <c r="E19">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4369,7 +4484,7 @@
         <v>101</v>
       </c>
       <c r="E20">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4389,7 +4504,7 @@
         <v>101</v>
       </c>
       <c r="E21">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4409,7 +4524,7 @@
         <v>95.5</v>
       </c>
       <c r="E22">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4429,7 +4544,7 @@
         <v>98.5</v>
       </c>
       <c r="E23">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4449,7 +4564,7 @@
         <v>87</v>
       </c>
       <c r="E24">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4469,7 +4584,7 @@
         <v>86.5</v>
       </c>
       <c r="E25">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4489,7 +4604,7 @@
         <v>86.5</v>
       </c>
       <c r="E26">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4509,7 +4624,7 @@
         <v>87</v>
       </c>
       <c r="E27">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4529,7 +4644,7 @@
         <v>96.5</v>
       </c>
       <c r="E28">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4549,7 +4664,7 @@
         <v>88</v>
       </c>
       <c r="E29">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4569,7 +4684,7 @@
         <v>98</v>
       </c>
       <c r="E30">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4589,7 +4704,7 @@
         <v>103.5</v>
       </c>
       <c r="E31">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4609,7 +4724,7 @@
         <v>92.5</v>
       </c>
       <c r="E32">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4629,7 +4744,7 @@
         <v>90.5</v>
       </c>
       <c r="E33">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4649,7 +4764,7 @@
         <v>86.5</v>
       </c>
       <c r="E34">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4669,7 +4784,7 @@
         <v>84</v>
       </c>
       <c r="E35">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4689,7 +4804,7 @@
         <v>91</v>
       </c>
       <c r="E36">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4709,7 +4824,7 @@
         <v>88</v>
       </c>
       <c r="E37">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4729,7 +4844,7 @@
         <v>100.5</v>
       </c>
       <c r="E38">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4749,7 +4864,7 @@
         <v>94</v>
       </c>
       <c r="E39">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4769,7 +4884,7 @@
         <v>105</v>
       </c>
       <c r="E40">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4789,7 +4904,7 @@
         <v>108</v>
       </c>
       <c r="E41">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4809,7 +4924,7 @@
         <v>84</v>
       </c>
       <c r="E42">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4829,7 +4944,7 @@
         <v>88.5</v>
       </c>
       <c r="E43">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4849,7 +4964,7 @@
         <v>91</v>
       </c>
       <c r="E44">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4869,7 +4984,7 @@
         <v>91</v>
       </c>
       <c r="E45">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4889,7 +5004,7 @@
         <v>92</v>
       </c>
       <c r="E46">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4909,7 +5024,7 @@
         <v>95.5</v>
       </c>
       <c r="E47">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4929,7 +5044,7 @@
         <v>108</v>
       </c>
       <c r="E48">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4949,7 +5064,7 @@
         <v>90.5</v>
       </c>
       <c r="E49">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4969,7 +5084,7 @@
         <v>98</v>
       </c>
       <c r="E50">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -4989,7 +5104,7 @@
         <v>99.5</v>
       </c>
       <c r="E51">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5009,7 +5124,7 @@
         <v>91</v>
       </c>
       <c r="E52">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5029,7 +5144,7 @@
         <v>88</v>
       </c>
       <c r="E53">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5049,7 +5164,7 @@
         <v>88</v>
       </c>
       <c r="E54">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5069,7 +5184,7 @@
         <v>85.5</v>
       </c>
       <c r="E55">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5089,7 +5204,7 @@
         <v>91</v>
       </c>
       <c r="E56">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5109,7 +5224,7 @@
         <v>92.5</v>
       </c>
       <c r="E57">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5129,7 +5244,7 @@
         <v>105</v>
       </c>
       <c r="E58">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5149,7 +5264,7 @@
         <v>90</v>
       </c>
       <c r="E59">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5169,7 +5284,7 @@
         <v>105</v>
       </c>
       <c r="E60">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5189,7 +5304,7 @@
         <v>98</v>
       </c>
       <c r="E61">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5209,7 +5324,7 @@
         <v>91</v>
       </c>
       <c r="E62">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5229,7 +5344,7 @@
         <v>93.5</v>
       </c>
       <c r="E63">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5249,7 +5364,7 @@
         <v>89.5</v>
       </c>
       <c r="E64">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5269,7 +5384,7 @@
         <v>91</v>
       </c>
       <c r="E65">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5289,7 +5404,7 @@
         <v>88.5</v>
       </c>
       <c r="E66">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -5305,17 +5420,17 @@
         <v>95</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D101" si="2">((B67+C67)/2)</f>
+        <f t="shared" ref="D67:D101" si="3">((B67+C67)/2)</f>
         <v>95</v>
       </c>
       <c r="E67">
-        <f>81</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" ref="A68:A101" si="3">A67+1</f>
+        <f t="shared" ref="A68:A101" si="4">A67+1</f>
         <v>66</v>
       </c>
       <c r="B68">
@@ -5325,17 +5440,17 @@
         <v>115</v>
       </c>
       <c r="D68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105.5</v>
       </c>
       <c r="E68">
-        <f>81</f>
+        <f t="shared" ref="E68:E101" si="5">MIN(E67,MIN(B68:C68))</f>
         <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="B69">
@@ -5345,17 +5460,17 @@
         <v>96</v>
       </c>
       <c r="D69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98.5</v>
       </c>
       <c r="E69">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="B70">
@@ -5365,17 +5480,17 @@
         <v>121</v>
       </c>
       <c r="D70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>106.5</v>
       </c>
       <c r="E70">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="B71">
@@ -5385,17 +5500,17 @@
         <v>112</v>
       </c>
       <c r="D71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>99.5</v>
       </c>
       <c r="E71">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="B72">
@@ -5405,17 +5520,17 @@
         <v>87</v>
       </c>
       <c r="D72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>91.5</v>
       </c>
       <c r="E72">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="B73">
@@ -5425,17 +5540,17 @@
         <v>86</v>
       </c>
       <c r="D73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>93.5</v>
       </c>
       <c r="E73">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="B74">
@@ -5445,17 +5560,17 @@
         <v>81</v>
       </c>
       <c r="D74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86.5</v>
       </c>
       <c r="E74">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="B75">
@@ -5465,17 +5580,17 @@
         <v>81</v>
       </c>
       <c r="D75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88</v>
       </c>
       <c r="E75">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="B76">
@@ -5485,17 +5600,17 @@
         <v>87</v>
       </c>
       <c r="D76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>91.5</v>
       </c>
       <c r="E76">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
       <c r="B77">
@@ -5505,17 +5620,17 @@
         <v>95</v>
       </c>
       <c r="D77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>95</v>
       </c>
       <c r="E77">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>76</v>
       </c>
       <c r="B78">
@@ -5525,17 +5640,17 @@
         <v>115</v>
       </c>
       <c r="D78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105.5</v>
       </c>
       <c r="E78">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
       <c r="B79">
@@ -5545,17 +5660,17 @@
         <v>90</v>
       </c>
       <c r="D79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>92.5</v>
       </c>
       <c r="E79">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78</v>
       </c>
       <c r="B80">
@@ -5565,17 +5680,17 @@
         <v>115</v>
       </c>
       <c r="D80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105.5</v>
       </c>
       <c r="E80">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>79</v>
       </c>
       <c r="B81">
@@ -5585,17 +5700,17 @@
         <v>106</v>
       </c>
       <c r="D81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100.5</v>
       </c>
       <c r="E81">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="B82">
@@ -5605,17 +5720,17 @@
         <v>101</v>
       </c>
       <c r="D82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="E82">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>81</v>
       </c>
       <c r="B83">
@@ -5625,17 +5740,17 @@
         <v>87</v>
       </c>
       <c r="D83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="E83">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="B84">
@@ -5645,17 +5760,17 @@
         <v>96</v>
       </c>
       <c r="D84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="E84">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83</v>
       </c>
       <c r="B85">
@@ -5665,297 +5780,297 @@
         <v>96</v>
       </c>
       <c r="D85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98.5</v>
       </c>
       <c r="E85">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
+        <f t="shared" si="4"/>
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>87</v>
+      </c>
+      <c r="C86">
+        <v>95</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <f t="shared" si="4"/>
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>90</v>
+      </c>
+      <c r="C87">
+        <v>90</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <f t="shared" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>81</v>
+      </c>
+      <c r="C88">
+        <v>124</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="3"/>
+        <v>102.5</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f t="shared" si="4"/>
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>87</v>
+      </c>
+      <c r="C89">
+        <v>87</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <f t="shared" si="4"/>
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>81</v>
+      </c>
+      <c r="C90">
+        <v>121</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="3"/>
+        <v>101</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <f t="shared" si="4"/>
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>86</v>
+      </c>
+      <c r="C91">
+        <v>121</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="3"/>
+        <v>103.5</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>87</v>
+      </c>
+      <c r="C92">
+        <v>95</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <f t="shared" si="4"/>
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>87</v>
+      </c>
+      <c r="C93">
+        <v>96</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="3"/>
+        <v>91.5</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <f t="shared" si="4"/>
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>95</v>
+      </c>
+      <c r="C94">
+        <v>87</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <f t="shared" si="4"/>
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>90</v>
+      </c>
+      <c r="C95">
+        <v>87</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="3"/>
+        <v>88.5</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <f t="shared" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96">
+        <v>92</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="3"/>
+        <v>93.5</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>87</v>
+      </c>
+      <c r="C97">
+        <v>87</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>96</v>
+      </c>
+      <c r="C98">
+        <v>112</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="3"/>
+        <v>104</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <f t="shared" si="4"/>
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>87</v>
+      </c>
+      <c r="C99">
+        <v>81</v>
+      </c>
+      <c r="D99">
         <f t="shared" si="3"/>
         <v>84</v>
       </c>
-      <c r="B86">
-        <v>87</v>
-      </c>
-      <c r="C86">
-        <v>95</v>
-      </c>
-      <c r="D86">
-        <f t="shared" si="2"/>
-        <v>91</v>
-      </c>
-      <c r="E86">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <f t="shared" si="3"/>
-        <v>85</v>
-      </c>
-      <c r="B87">
-        <v>90</v>
-      </c>
-      <c r="C87">
-        <v>90</v>
-      </c>
-      <c r="D87">
-        <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="E87">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <f t="shared" si="3"/>
-        <v>86</v>
-      </c>
-      <c r="B88">
-        <v>81</v>
-      </c>
-      <c r="C88">
-        <v>124</v>
-      </c>
-      <c r="D88">
-        <f t="shared" si="2"/>
-        <v>102.5</v>
-      </c>
-      <c r="E88">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <f t="shared" si="3"/>
-        <v>87</v>
-      </c>
-      <c r="B89">
-        <v>87</v>
-      </c>
-      <c r="C89">
-        <v>87</v>
-      </c>
-      <c r="D89">
-        <f t="shared" si="2"/>
-        <v>87</v>
-      </c>
-      <c r="E89">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <f t="shared" si="3"/>
-        <v>88</v>
-      </c>
-      <c r="B90">
-        <v>81</v>
-      </c>
-      <c r="C90">
-        <v>121</v>
-      </c>
-      <c r="D90">
-        <f t="shared" si="2"/>
-        <v>101</v>
-      </c>
-      <c r="E90">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <f t="shared" si="3"/>
-        <v>89</v>
-      </c>
-      <c r="B91">
-        <v>86</v>
-      </c>
-      <c r="C91">
-        <v>121</v>
-      </c>
-      <c r="D91">
-        <f t="shared" si="2"/>
-        <v>103.5</v>
-      </c>
-      <c r="E91">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <f t="shared" si="3"/>
-        <v>90</v>
-      </c>
-      <c r="B92">
-        <v>87</v>
-      </c>
-      <c r="C92">
-        <v>95</v>
-      </c>
-      <c r="D92">
-        <f t="shared" si="2"/>
-        <v>91</v>
-      </c>
-      <c r="E92">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <f t="shared" si="3"/>
-        <v>91</v>
-      </c>
-      <c r="B93">
-        <v>87</v>
-      </c>
-      <c r="C93">
-        <v>96</v>
-      </c>
-      <c r="D93">
-        <f t="shared" si="2"/>
-        <v>91.5</v>
-      </c>
-      <c r="E93">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <f t="shared" si="3"/>
-        <v>92</v>
-      </c>
-      <c r="B94">
-        <v>95</v>
-      </c>
-      <c r="C94">
-        <v>87</v>
-      </c>
-      <c r="D94">
-        <f t="shared" si="2"/>
-        <v>91</v>
-      </c>
-      <c r="E94">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <f t="shared" si="3"/>
-        <v>93</v>
-      </c>
-      <c r="B95">
-        <v>90</v>
-      </c>
-      <c r="C95">
-        <v>87</v>
-      </c>
-      <c r="D95">
-        <f t="shared" si="2"/>
-        <v>88.5</v>
-      </c>
-      <c r="E95">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <f t="shared" si="3"/>
-        <v>94</v>
-      </c>
-      <c r="B96">
-        <v>95</v>
-      </c>
-      <c r="C96">
-        <v>92</v>
-      </c>
-      <c r="D96">
-        <f t="shared" si="2"/>
-        <v>93.5</v>
-      </c>
-      <c r="E96">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <f t="shared" si="3"/>
-        <v>95</v>
-      </c>
-      <c r="B97">
-        <v>87</v>
-      </c>
-      <c r="C97">
-        <v>87</v>
-      </c>
-      <c r="D97">
-        <f t="shared" si="2"/>
-        <v>87</v>
-      </c>
-      <c r="E97">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <f t="shared" si="3"/>
-        <v>96</v>
-      </c>
-      <c r="B98">
-        <v>96</v>
-      </c>
-      <c r="C98">
-        <v>112</v>
-      </c>
-      <c r="D98">
-        <f t="shared" si="2"/>
-        <v>104</v>
-      </c>
-      <c r="E98">
-        <f>81</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <f t="shared" si="3"/>
-        <v>97</v>
-      </c>
-      <c r="B99">
-        <v>87</v>
-      </c>
-      <c r="C99">
-        <v>81</v>
-      </c>
-      <c r="D99">
-        <f t="shared" si="2"/>
-        <v>84</v>
-      </c>
       <c r="E99">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
       <c r="B100">
@@ -5965,17 +6080,17 @@
         <v>115</v>
       </c>
       <c r="D100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="E100">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
       <c r="B101">
@@ -5985,11 +6100,11 @@
         <v>121</v>
       </c>
       <c r="D101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105.5</v>
       </c>
       <c r="E101">
-        <f>81</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>

</xml_diff>